<commit_message>
correct sign error in ZD and reinstated az_to_tz function as we need this now for exporting to csv. Add functions to make bottle sheet by drawing in data from a ctd sheet and ros bottle files. Added more extdata. Remove copy of read_elg in this package and will rely on claling it from the sea package. For now.
</commit_message>
<xml_diff>
--- a/inst/extdata/S285_station.xlsx
+++ b/inst/extdata/S285_station.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19580" windowHeight="21100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="73">
   <si>
     <t>station</t>
   </si>
@@ -27,9 +27,6 @@
     <t>deployment</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -138,15 +135,6 @@
     <t>S285-017</t>
   </si>
   <si>
-    <t>ctd</t>
-  </si>
-  <si>
-    <t>+13</t>
-  </si>
-  <si>
-    <t>-11</t>
-  </si>
-  <si>
     <t>2019-04-01</t>
   </si>
   <si>
@@ -172,6 +160,84 @@
   </si>
   <si>
     <t>2019-04-09</t>
+  </si>
+  <si>
+    <t>time_in</t>
+  </si>
+  <si>
+    <t>time_out</t>
+  </si>
+  <si>
+    <t>00:00</t>
+  </si>
+  <si>
+    <t>CTD</t>
+  </si>
+  <si>
+    <t>NT</t>
+  </si>
+  <si>
+    <t>12:13</t>
+  </si>
+  <si>
+    <t>12:44</t>
+  </si>
+  <si>
+    <t>12:14</t>
+  </si>
+  <si>
+    <t>00:01</t>
+  </si>
+  <si>
+    <t>00:31</t>
+  </si>
+  <si>
+    <t>11:45</t>
+  </si>
+  <si>
+    <t>12:15</t>
+  </si>
+  <si>
+    <t>00:07</t>
+  </si>
+  <si>
+    <t>11:11</t>
+  </si>
+  <si>
+    <t>11:41</t>
+  </si>
+  <si>
+    <t>23:02</t>
+  </si>
+  <si>
+    <t>23:33</t>
+  </si>
+  <si>
+    <t>-13</t>
+  </si>
+  <si>
+    <t>+11</t>
+  </si>
+  <si>
+    <t>00:04</t>
+  </si>
+  <si>
+    <t>00:34</t>
+  </si>
+  <si>
+    <t>12:06</t>
+  </si>
+  <si>
+    <t>12:37</t>
+  </si>
+  <si>
+    <t>23:48</t>
+  </si>
+  <si>
+    <t>00:18</t>
+  </si>
+  <si>
+    <t>12:04</t>
   </si>
 </sst>
 </file>
@@ -225,8 +291,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -248,13 +344,43 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -584,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -595,7 +721,7 @@
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1">
+    <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -603,306 +729,547 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="D21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="D26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="2">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="2">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="2">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="3" t="s">
+      <c r="D27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="B28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="2">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="2">
-        <v>-11</v>
+      <c r="E28" s="3"/>
+      <c r="F28" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
add beginning of extra neuston processing. Currently have ability to extract tow distance although need to verify this is being done correctly
</commit_message>
<xml_diff>
--- a/inst/extdata/S285_station.xlsx
+++ b/inst/extdata/S285_station.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19580" windowHeight="21100" tabRatio="500"/>
+    <workbookView xWindow="22480" yWindow="1140" windowWidth="19580" windowHeight="21100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="74">
   <si>
     <t>station</t>
   </si>
@@ -168,9 +168,6 @@
     <t>time_out</t>
   </si>
   <si>
-    <t>00:00</t>
-  </si>
-  <si>
     <t>CTD</t>
   </si>
   <si>
@@ -238,13 +235,19 @@
   </si>
   <si>
     <t>12:04</t>
+  </si>
+  <si>
+    <t>00:05</t>
+  </si>
+  <si>
+    <t>11:34</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -271,6 +274,12 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -713,7 +722,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -746,7 +755,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>38</v>
@@ -755,10 +764,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -766,7 +775,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>39</v>
@@ -776,7 +785,7 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -784,19 +793,19 @@
         <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -804,7 +813,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>39</v>
@@ -812,9 +821,11 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="F5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -822,7 +833,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>40</v>
@@ -832,7 +843,7 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -840,7 +851,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>40</v>
@@ -850,7 +861,7 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -858,19 +869,19 @@
         <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -878,7 +889,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>40</v>
@@ -888,7 +899,7 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -896,19 +907,19 @@
         <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -916,7 +927,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>41</v>
@@ -926,7 +937,7 @@
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -934,19 +945,19 @@
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -954,7 +965,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>41</v>
@@ -963,10 +974,10 @@
         <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -974,7 +985,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>42</v>
@@ -984,7 +995,7 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -992,19 +1003,19 @@
         <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1012,7 +1023,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>42</v>
@@ -1022,7 +1033,7 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1030,19 +1041,19 @@
         <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1050,7 +1061,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>43</v>
@@ -1060,7 +1071,7 @@
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1068,7 +1079,7 @@
         <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>43</v>
@@ -1078,7 +1089,7 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1086,19 +1097,19 @@
         <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1106,7 +1117,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>44</v>
@@ -1116,7 +1127,7 @@
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1124,19 +1135,19 @@
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1144,7 +1155,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>44</v>
@@ -1154,7 +1165,7 @@
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1162,19 +1173,19 @@
         <v>34</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1182,7 +1193,7 @@
         <v>35</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>45</v>
@@ -1192,7 +1203,7 @@
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1200,7 +1211,7 @@
         <v>36</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>46</v>
@@ -1210,7 +1221,7 @@
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1218,17 +1229,19 @@
         <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F27" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1236,7 +1249,7 @@
         <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>46</v>
@@ -1246,7 +1259,7 @@
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1254,22 +1267,24 @@
         <v>37</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="F29" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>